<commit_message>
New Bill Payment Push
</commit_message>
<xml_diff>
--- a/Test Data/Bill.xlsx
+++ b/Test Data/Bill.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>biller</t>
   </si>
@@ -39,16 +39,25 @@
     <t>SalikPIN</t>
   </si>
   <si>
-    <t>011000186020</t>
-  </si>
-  <si>
     <t>FEWA</t>
   </si>
   <si>
     <t>partial</t>
   </si>
   <si>
-    <t>011000186018</t>
+    <t>Du</t>
+  </si>
+  <si>
+    <t>du Postpaid</t>
+  </si>
+  <si>
+    <t>ADDC</t>
+  </si>
+  <si>
+    <t>011074763011</t>
+  </si>
+  <si>
+    <t>011074763023</t>
   </si>
 </sst>
 </file>
@@ -397,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -438,10 +447,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5">
         <v>210000137777</v>
@@ -450,30 +459,44 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5">
-        <v>210000137777</v>
+        <v>599588538</v>
       </c>
       <c r="D3" s="6">
         <v>100</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5">
+        <v>8235355929</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>